<commit_message>
update h2 inputs with new SMR designs
</commit_message>
<xml_diff>
--- a/code/SMR_inputs.xlsx
+++ b/code/SMR_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgarrous/Documents/SMR_deployment/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4828A53B-F449-9E41-91EC-F88897AE14CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F36D40-F0D7-1045-94A1-66B0C04DE9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="1240" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="1440" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FOAK_act" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>Reactor</t>
+    <t>Type</t>
   </si>
   <si>
     <t>Power in MWe</t>
@@ -468,7 +468,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>